<commit_message>
Working User Groups and Group Members Unity Interfaces
</commit_message>
<xml_diff>
--- a/Unity/Assets/SUGAR/Resources/Localization/SUGAR Unity Localization.xlsx
+++ b/Unity/Assets/SUGAR/Resources/Localization/SUGAR Unity Localization.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="92">
   <si>
     <t>Key</t>
   </si>
@@ -100,7 +100,7 @@
     <t>FRIENDS_PENDING_SENT</t>
   </si>
   <si>
-    <t>Sent Friends Requests</t>
+    <t>Sent Friend Requests</t>
   </si>
   <si>
     <t>GROUP</t>
@@ -121,16 +121,22 @@
     <t>Groups</t>
   </si>
   <si>
+    <t>GROUPS_LOAD_ERROR</t>
+  </si>
+  <si>
+    <t>Error: Unable to gather list of groups.</t>
+  </si>
+  <si>
     <t>GROUPS_PENDING_REQUESTS</t>
   </si>
   <si>
     <t>Group Requests</t>
   </si>
   <si>
-    <t>GROUPS_PENDING_SENT</t>
-  </si>
-  <si>
-    <t>Sent Group Requests</t>
+    <t>PENDING_SENT</t>
+  </si>
+  <si>
+    <t>Sent Requests</t>
   </si>
   <si>
     <t>LEADERBOARD_LIST_LOAD_ERROR</t>
@@ -278,6 +284,9 @@
   </si>
   <si>
     <t>Score</t>
+  </si>
+  <si>
+    <t>Error: Unable to gather list of group members.</t>
   </si>
 </sst>
 </file>
@@ -332,7 +341,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -990,66 +999,66 @@
         <v>47</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21">
@@ -1305,31 +1314,31 @@
         <v>66</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29">
@@ -1340,31 +1349,31 @@
         <v>68</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30">
@@ -1480,31 +1489,31 @@
         <v>76</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34">
@@ -1515,31 +1524,31 @@
         <v>78</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35">
@@ -1714,6 +1723,76 @@
         <v>13</v>
       </c>
       <c r="K39" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K41" s="2" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update dlls  for text localization to be imported correctly add remember me to the default sugar unity localizations
</commit_message>
<xml_diff>
--- a/Unity/Assets/SUGAR/Resources/Localization/SUGAR Unity Localization.xlsx
+++ b/Unity/Assets/SUGAR/Resources/Localization/SUGAR Unity Localization.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Documents\Projects\sugar-unity\Unity\Assets\SUGAR\Resources\Localization\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="510" yWindow="600" windowWidth="24615" windowHeight="11955"/>
+    <workbookView xWindow="510" yWindow="600" windowWidth="24620" windowHeight="11960"/>
   </bookViews>
   <sheets>
     <sheet name="SUGARLocalizations" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="87">
   <si>
     <t>Key</t>
   </si>
@@ -269,6 +274,12 @@
   </si>
   <si>
     <t>Alliances</t>
+  </si>
+  <si>
+    <t>REMEMBER</t>
+  </si>
+  <si>
+    <t>Remember Me</t>
   </si>
 </sst>
 </file>
@@ -324,6 +335,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -371,7 +385,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -406,7 +420,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -615,22 +629,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B34" sqref="B34"/>
+      <selection pane="bottomRight" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" customWidth="1"/>
+    <col min="1" max="1" width="33.7265625" customWidth="1"/>
     <col min="2" max="2" width="58" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -647,7 +661,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -664,7 +678,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -681,7 +695,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -698,7 +712,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -715,7 +729,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -732,7 +746,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -749,7 +763,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -766,7 +780,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -783,7 +797,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -800,7 +814,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -817,7 +831,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -834,7 +848,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -851,7 +865,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
@@ -868,7 +882,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
@@ -885,7 +899,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>28</v>
       </c>
@@ -902,7 +916,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>30</v>
       </c>
@@ -919,7 +933,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>32</v>
       </c>
@@ -936,7 +950,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>34</v>
       </c>
@@ -953,7 +967,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>36</v>
       </c>
@@ -970,7 +984,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>38</v>
       </c>
@@ -987,7 +1001,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>40</v>
       </c>
@@ -1004,7 +1018,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>42</v>
       </c>
@@ -1021,7 +1035,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>44</v>
       </c>
@@ -1038,7 +1052,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>46</v>
       </c>
@@ -1055,7 +1069,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>48</v>
       </c>
@@ -1072,7 +1086,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>50</v>
       </c>
@@ -1089,7 +1103,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>52</v>
       </c>
@@ -1106,7 +1120,7 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>54</v>
       </c>
@@ -1123,7 +1137,7 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>56</v>
       </c>
@@ -1140,7 +1154,7 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>58</v>
       </c>
@@ -1157,7 +1171,7 @@
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>60</v>
       </c>
@@ -1174,7 +1188,7 @@
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>62</v>
       </c>
@@ -1191,7 +1205,7 @@
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>64</v>
       </c>
@@ -1208,12 +1222,12 @@
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>67</v>
+    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1225,12 +1239,12 @@
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -1242,12 +1256,12 @@
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -1259,12 +1273,12 @@
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
     </row>
-    <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -1276,12 +1290,12 @@
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -1293,12 +1307,12 @@
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -1310,12 +1324,12 @@
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -1327,19 +1341,36 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix for streaming assets config file being required for seeding. Updated localization to match text required in DLL scripts, example scripts and provided UI.
</commit_message>
<xml_diff>
--- a/Unity/Assets/SUGAR/Resources/Localization/SUGAR Unity Localization.xlsx
+++ b/Unity/Assets/SUGAR/Resources/Localization/SUGAR Unity Localization.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Documents\Projects\sugar-unity\Unity\Assets\SUGAR\Resources\Localization\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="510" yWindow="600" windowWidth="24620" windowHeight="11960"/>
+    <workbookView xWindow="510" yWindow="600" windowWidth="24615" windowHeight="11955"/>
   </bookViews>
   <sheets>
     <sheet name="SUGARLocalizations" sheetId="1" r:id="rId1"/>
@@ -19,17 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>Key</t>
   </si>
   <si>
-    <t>ACHIEVEMENT_LOAD_ERROR</t>
-  </si>
-  <si>
-    <t>Error: Unable to gather current achievement progress.</t>
-  </si>
-  <si>
     <t>ACHIEVEMENTS</t>
   </si>
   <si>
@@ -63,9 +52,6 @@
     <t>FRIENDS_LOAD_ERROR</t>
   </si>
   <si>
-    <t>Error: Unable to gather list of users.</t>
-  </si>
-  <si>
     <t>FRIENDS_PENDING_REQUESTS</t>
   </si>
   <si>
@@ -93,24 +79,9 @@
     <t>Groups</t>
   </si>
   <si>
-    <t>GROUPS_LOAD_ERROR</t>
-  </si>
-  <si>
-    <t>Error: Unable to gather list of groups.</t>
-  </si>
-  <si>
     <t>GROUPS_PENDING_REQUESTS</t>
   </si>
   <si>
-    <t>Group Requests</t>
-  </si>
-  <si>
-    <t>PENDING_SENT</t>
-  </si>
-  <si>
-    <t>Sent Requests</t>
-  </si>
-  <si>
     <t>LEADERBOARD_LIST_LOAD_ERROR</t>
   </si>
   <si>
@@ -141,24 +112,12 @@
     <t>Near</t>
   </si>
   <si>
-    <t>NEARBY</t>
-  </si>
-  <si>
-    <t>Nearby</t>
-  </si>
-  <si>
     <t>NEXT</t>
   </si>
   <si>
     <t>Next</t>
   </si>
   <si>
-    <t>NO_ACHIEVEMENT_ERROR</t>
-  </si>
-  <si>
-    <t>No achievements are currently available for this game.</t>
-  </si>
-  <si>
     <t>NO_LEADERBOARD_ERROR</t>
   </si>
   <si>
@@ -258,15 +217,9 @@
     <t>Error: Unable to gather list of group members.</t>
   </si>
   <si>
-    <t>Friend Requests</t>
-  </si>
-  <si>
     <t>en</t>
   </si>
   <si>
-    <t>GROUP_MEMBERS</t>
-  </si>
-  <si>
     <t>ALLIANCES</t>
   </si>
   <si>
@@ -280,6 +233,57 @@
   </si>
   <si>
     <t>Remember Me</t>
+  </si>
+  <si>
+    <t>EVALUATION_LOAD_ERROR</t>
+  </si>
+  <si>
+    <t>NO_EVALUATION_ERROR</t>
+  </si>
+  <si>
+    <t>Error: Unable to gather current progress.</t>
+  </si>
+  <si>
+    <t>No progress is currently tracked for this game.</t>
+  </si>
+  <si>
+    <t>Error: Unable to gather friend data.</t>
+  </si>
+  <si>
+    <t>USER_GROUPS_LOAD_ERROR</t>
+  </si>
+  <si>
+    <t>Error: Unable to gather group data for this user.</t>
+  </si>
+  <si>
+    <t>GROUPS_MEMBER_LOAD_ERROR</t>
+  </si>
+  <si>
+    <t>GROUPMEMBERS</t>
+  </si>
+  <si>
+    <t>SKILLS</t>
+  </si>
+  <si>
+    <t>Skills</t>
+  </si>
+  <si>
+    <t>Received Friend Requests</t>
+  </si>
+  <si>
+    <t>Received Group Requests</t>
+  </si>
+  <si>
+    <t>GROUPS_PENDING_SENT</t>
+  </si>
+  <si>
+    <t>Sent Group Requests</t>
+  </si>
+  <si>
+    <t>SHOW_ME</t>
+  </si>
+  <si>
+    <t>Show Me</t>
   </si>
 </sst>
 </file>
@@ -321,10 +325,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,7 +391,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -420,7 +426,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -629,27 +635,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B35" sqref="B35"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.7265625" customWidth="1"/>
+    <col min="1" max="1" width="33.7109375" customWidth="1"/>
     <col min="2" max="2" width="58" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -661,8 +667,8 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -678,12 +684,12 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -695,12 +701,12 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -712,12 +718,12 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -729,12 +735,12 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -746,12 +752,12 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>11</v>
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -763,12 +769,12 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -780,12 +786,12 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>15</v>
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -797,12 +803,12 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>17</v>
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -814,12 +820,12 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>18</v>
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -831,12 +837,12 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>20</v>
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -848,12 +854,12 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>22</v>
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -865,12 +871,12 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>25</v>
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -882,12 +888,12 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>26</v>
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -899,12 +905,12 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>28</v>
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -916,12 +922,12 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>31</v>
+    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -933,12 +939,12 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>33</v>
+    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -950,12 +956,12 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>34</v>
+    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -967,12 +973,12 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>36</v>
+    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -984,12 +990,12 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>38</v>
+    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1001,12 +1007,12 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>40</v>
+    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1018,12 +1024,12 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>42</v>
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1035,12 +1041,12 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>45</v>
+    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1052,12 +1058,12 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>46</v>
+    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1069,12 +1075,12 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>49</v>
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1086,12 +1092,12 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>51</v>
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1103,12 +1109,12 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>52</v>
+    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1120,12 +1126,12 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>55</v>
+    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1137,12 +1143,12 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>56</v>
+    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -1154,12 +1160,12 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>58</v>
+    <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1171,12 +1177,12 @@
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>60</v>
+    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1188,12 +1194,12 @@
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>62</v>
+    <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1205,12 +1211,12 @@
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>64</v>
+    <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -1222,12 +1228,12 @@
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>86</v>
+    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1239,12 +1245,12 @@
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>67</v>
+    <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -1256,12 +1262,12 @@
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>69</v>
+    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -1273,12 +1279,12 @@
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
     </row>
-    <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>70</v>
+    <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -1290,12 +1296,12 @@
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>72</v>
+    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -1307,12 +1313,12 @@
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>75</v>
+    <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -1324,12 +1330,12 @@
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>76</v>
+    <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -1341,40 +1347,42 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>24</v>
+    <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-    </row>
-    <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="B43" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:B46">
+    <sortCondition ref="A2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>